<commit_message>
update to latest excel tool
</commit_message>
<xml_diff>
--- a/rawresource/rawconfig/ai.xlsx
+++ b/rawresource/rawconfig/ai.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0">
+    <comment ref="C2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -40,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0">
+    <comment ref="F2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -59,17 +59,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
-  <si>
-    <t xml:space="preserve">道具配置</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+  <si>
+    <t xml:space="preserve">ai_base_conf</t>
   </si>
   <si>
     <t xml:space="preserve">怪物AI配置</t>
   </si>
   <si>
-    <t xml:space="preserve">array</t>
-  </si>
-  <si>
     <t xml:space="preserve">唯一id</t>
   </si>
   <si>
@@ -85,13 +82,13 @@
     <t xml:space="preserve">其他AI参数</t>
   </si>
   <si>
-    <t xml:space="preserve">int</t>
+    <t xml:space="preserve">num</t>
   </si>
   <si>
     <t xml:space="preserve">lua</t>
   </si>
   <si>
-    <t xml:space="preserve">server</t>
+    <t xml:space="preserve">s</t>
   </si>
   <si>
     <t xml:space="preserve">id</t>
@@ -109,7 +106,7 @@
     <t xml:space="preserve">param</t>
   </si>
   <si>
-    <t xml:space="preserve">client</t>
+    <t xml:space="preserve">后端用来测试的AI</t>
   </si>
   <si>
     <t xml:space="preserve">{login_time = 600,logout_time = 1200}</t>
@@ -185,19 +182,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -268,11 +262,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -291,12 +281,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -362,166 +352,162 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="92.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="92.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.75"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="n">
+        <v>10001</v>
+      </c>
+      <c r="C7" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C8" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="n">
-        <v>10001</v>
-      </c>
-      <c r="C8" s="1" t="n">
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <v>20001</v>
+      </c>
+      <c r="C9" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="n">
-        <v>20000</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1" t="n">
-        <v>20001</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="n">
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="0" t="n">
         <v>40</v>
       </c>
     </row>
@@ -538,29 +524,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A4:J32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I44" activeCellId="0" sqref="I44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,7 +553,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -576,7 +561,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -584,112 +569,112 @@
         <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="J21" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="J21" s="0" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>